<commit_message>
Adding CSGO custom botting.
</commit_message>
<xml_diff>
--- a/GModSpecificResources/SuperiorServers/sup_gmod_commands.xlsx
+++ b/GModSpecificResources/SuperiorServers/sup_gmod_commands.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="245">
   <si>
     <t xml:space="preserve">COMMAND</t>
   </si>
@@ -65,10 +65,10 @@
     <t xml:space="preserve">/bail</t>
   </si>
   <si>
-    <t xml:space="preserve">Anyone?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bail someone out of jail. You may have to be looking at the bail machine in PD</t>
+    <t xml:space="preserve">Anyone? Mayor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bail someone out of jail. You may have to be looking at the bail machine in PD. If you’re the Mayor the price is free but you must be near your computer.</t>
   </si>
   <si>
     <t xml:space="preserve">/channel [number]</t>
@@ -338,6 +338,9 @@
     <t xml:space="preserve">/playercolor [red] [green] [blue]</t>
   </si>
   <si>
+    <t xml:space="preserve">Anyone?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Change your color to rgb blends?</t>
   </si>
   <si>
@@ -503,6 +506,21 @@
     <t xml:space="preserve">Command is valid yet currently unknown</t>
   </si>
   <si>
+    <t xml:space="preserve">/buyseed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug Dealers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buys 1 marijuana seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/buy [shop item]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase the item from general shop</t>
+  </si>
+  <si>
     <t xml:space="preserve">/citizen</t>
   </si>
   <si>
@@ -515,19 +533,239 @@
     <t xml:space="preserve">Switch classes to a Free Runner</t>
   </si>
   <si>
-    <t xml:space="preserve">/buyseed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drug Dealers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buys 1 marijuana seed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/buy [shop item]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase the item from general shop</t>
+    <t xml:space="preserve">/rapist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIP Members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Rapist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/protester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Protester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Staff On Duty (SOD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/hitman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Hitman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/prostitute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Prostitute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/pimp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Pimp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/hotelmanager</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Switch classes to a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Hotel Manager</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">/dj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a DJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/cinemaowner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Cinema Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/casinoowner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Casino Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/police</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Police</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/policechief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Police Chief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/hacker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Hacker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/rentacop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Rent-A-Cop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/merc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Mercenary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/hoboking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Hobo King</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/hobo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Hobo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/methhead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Meth Head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/gundealer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Gun Dealer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/blackmarketdealer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Black Market Dealer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/drugdealer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Drug Dealer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/bartender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Bartender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/cook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Cook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/medic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Medic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/mobboss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Mob Boss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/gangster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Gangster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/thug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Thug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/prothief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Pro Thief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/thief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Thief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/anarchist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch classes to a Anarchist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prostitutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offer sex to the person you’re looking at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/mayor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register a vote to be the next mayor if there is not one already</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/copbuy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase items from the “Cop Shop”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/laws</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prompts a text box to change current laws (Only runs when near office computer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/lotto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starts a lotto that you will get a 5% cut from. (Only runs when near office computer)</t>
   </si>
   <si>
     <t xml:space="preserve">Mods please sticky!</t>
@@ -570,7 +808,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -606,6 +844,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -671,7 +914,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -688,15 +931,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -777,12 +1024,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+      <selection pane="bottomLeft" activeCell="C116" activeCellId="0" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1236,343 +1483,728 @@
         <v>95</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>47</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>17</v>
+        <v>153</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1593,7 +2225,7 @@
   </sheetPr>
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1604,67 +2236,67 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>160</v>
+      <c r="A1" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>161</v>
+      <c r="A3" s="6" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>162</v>
+      <c r="A5" s="7" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>163</v>
+      <c r="A6" s="5" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>164</v>
+      <c r="A7" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>165</v>
+      <c r="A8" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>166</v>
+      <c r="A9" s="5" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>167</v>
+      <c r="A10" s="5" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>168</v>
+      <c r="A11" s="5" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>169</v>
+      <c r="A13" s="7" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>170</v>
+      <c r="A21" s="5" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added another launcher option
</commit_message>
<xml_diff>
--- a/GModSpecificResources/SuperiorServers/sup_gmod_commands.xlsx
+++ b/GModSpecificResources/SuperiorServers/sup_gmod_commands.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="258">
   <si>
     <t xml:space="preserve">COMMAND</t>
   </si>
@@ -344,6 +344,12 @@
     <t xml:space="preserve">Change your color to rgb blends?</t>
   </si>
   <si>
+    <t xml:space="preserve">/physcolor [red] [green] [blue]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes your physgun color to exact RGB values</t>
+  </si>
+  <si>
     <t xml:space="preserve">/act [action]</t>
   </si>
   <si>
@@ -521,6 +527,39 @@
     <t xml:space="preserve">Purchase the item from general shop</t>
   </si>
   <si>
+    <t xml:space="preserve">Purchases a weed seed from the F4 shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/buypot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases a weed pot from the F4 shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/buyinker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases a money printer upgrade from the F4 shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/buyprinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases a money printer from the F4 shop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/buyammo [type]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases a type of ammo from the F4 shop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/buyhealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases health from the F4 shop (Only when doctors aren't on) </t>
+  </si>
+  <si>
     <t xml:space="preserve">/citizen</t>
   </si>
   <si>
@@ -575,23 +614,7 @@
     <t xml:space="preserve">/hotelmanager</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Switch classes to a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Hotel Manager</t>
-    </r>
+    <t xml:space="preserve">Switch classes to a Hotel Manager</t>
   </si>
   <si>
     <t xml:space="preserve">/dj</t>
@@ -808,7 +831,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -844,11 +867,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -914,7 +932,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -931,19 +949,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1024,12 +1038,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C116" activeCellId="0" sqref="C116"/>
+      <selection pane="bottomLeft" activeCell="C76" activeCellId="0" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1505,7 +1519,7 @@
         <v>100</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>101</v>
@@ -1516,18 +1530,18 @@
         <v>102</v>
       </c>
       <c r="C41" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>106</v>
@@ -1537,22 +1551,22 @@
       <c r="A43" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="C43" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>110</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>111</v>
@@ -1563,7 +1577,7 @@
         <v>112</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>113</v>
@@ -1574,7 +1588,7 @@
         <v>114</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>115</v>
@@ -1585,7 +1599,7 @@
         <v>116</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>117</v>
@@ -1596,21 +1610,21 @@
         <v>118</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,9 +1632,9 @@
         <v>121</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1629,7 +1643,7 @@
         <v>123</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>124</v>
@@ -1640,9 +1654,9 @@
         <v>125</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1651,7 +1665,7 @@
         <v>127</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>128</v>
@@ -1662,7 +1676,7 @@
         <v>129</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>130</v>
@@ -1673,7 +1687,7 @@
         <v>131</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>132</v>
@@ -1684,7 +1698,7 @@
         <v>133</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>134</v>
@@ -1694,8 +1708,8 @@
       <c r="A57" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>103</v>
+      <c r="C57" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>136</v>
@@ -1705,8 +1719,8 @@
       <c r="A58" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>103</v>
+      <c r="C58" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>138</v>
@@ -1717,7 +1731,7 @@
         <v>139</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>140</v>
@@ -1728,7 +1742,7 @@
         <v>141</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>142</v>
@@ -1739,7 +1753,7 @@
         <v>143</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>144</v>
@@ -1750,7 +1764,7 @@
         <v>145</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>146</v>
@@ -1761,7 +1775,7 @@
         <v>147</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>148</v>
@@ -1772,29 +1786,29 @@
         <v>149</v>
       </c>
       <c r="C64" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="D65" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>156</v>
@@ -1813,398 +1827,475 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>165</v>
+      <c r="D70" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>167</v>
+        <v>17</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D72" s="4" t="s">
-        <v>169</v>
+      <c r="D72" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>171</v>
+      <c r="D73" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>173</v>
+        <v>17</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D75" s="4" t="s">
-        <v>175</v>
+      <c r="D75" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D76" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D99" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D100" s="0" t="s">
-        <v>226</v>
+      <c r="D100" s="3" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>228</v>
+        <v>17</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>231</v>
+        <v>17</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C103" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="D103" s="0" t="s">
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
         <v>233</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2236,67 +2327,67 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>234</v>
+      <c r="A1" s="4" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>235</v>
+      <c r="A3" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>236</v>
+      <c r="A5" s="6" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>237</v>
+      <c r="A6" s="4" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>238</v>
+      <c r="A7" s="4" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>239</v>
+      <c r="A8" s="4" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>240</v>
+      <c r="A9" s="4" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>241</v>
+      <c r="A10" s="4" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>242</v>
+      <c r="A11" s="4" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>243</v>
+      <c r="A13" s="6" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>244</v>
+      <c r="A21" s="4" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>